<commit_message>
Update SALN Reports Generation
</commit_message>
<xml_diff>
--- a/website/static/saln/modified_summary_list_of_filers_test.xlsx
+++ b/website/static/saln/modified_summary_list_of_filers_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="138">
   <si>
     <t>SUMMARY LIST OF FILERS</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>NET WORTH</t>
+  </si>
+  <si>
+    <t>AS OF</t>
   </si>
   <si>
     <t>PERMANENT</t>
@@ -436,6 +439,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mmm d, yyyy"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -528,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -553,6 +559,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -858,7 +867,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -873,9 +882,10 @@
     <col min="7" max="7" width="15.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="41.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -888,7 +898,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1">
+    <row r="2" spans="1:10" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -901,7 +911,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="22.5" customHeight="1">
+    <row r="3" spans="1:10" ht="22.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -914,7 +924,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1">
+    <row r="4" spans="1:10" s="5" customFormat="1">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -934,8 +944,11 @@
       <c r="I4" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
         <v>5</v>
@@ -951,10 +964,11 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -965,109 +979,121 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="9">
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>18</v>
+      </c>
+      <c r="J7" s="11">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="9">
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>24</v>
+      </c>
+      <c r="J8" s="11">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="9">
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>30</v>
+      </c>
+      <c r="J9" s="11">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="9">
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>35</v>
+      </c>
+      <c r="J10" s="11">
+        <v>45303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1078,59 +1104,65 @@
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="9">
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>42</v>
+      </c>
+      <c r="J12" s="11">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="9">
         <v>2</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>48</v>
+      </c>
+      <c r="J13" s="11">
+        <v>45307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1141,261 +1173,279 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="9">
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>55</v>
+      </c>
+      <c r="J15" s="11">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="9">
         <v>2</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>61</v>
+      </c>
+      <c r="J16" s="11">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="9">
         <v>3</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>67</v>
+      </c>
+      <c r="J17" s="11">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="9">
         <v>4</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>72</v>
+      </c>
+      <c r="J18" s="11">
+        <v>45310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="9">
         <v>5</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>77</v>
+      </c>
+      <c r="J19" s="11">
+        <v>45310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="9">
         <v>6</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="B22" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="12">
+      <c r="J20" s="11">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="B22" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="B23" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="12">
+    <row r="23" spans="1:10">
+      <c r="B23" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="B26" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="13" t="s">
+    <row r="26" spans="1:10">
+      <c r="B26" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="G30" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="B31" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="G31" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="13" customHeight="1">
+      <c r="B34" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="13" customHeight="1">
+      <c r="B35" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="13" customHeight="1">
+      <c r="B36" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="B30" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="G30" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H30" s="12"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="B31" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="G31" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H31" s="14"/>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="B33" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="11" t="s">
+      <c r="G36" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G33" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="13" customHeight="1">
-      <c r="B34" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="13" customHeight="1">
-      <c r="B35" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="13" customHeight="1">
-      <c r="B36" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>95</v>
+      <c r="H36" s="12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="13" customHeight="1"/>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
@@ -1405,6 +1455,7 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:H5"/>
     <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="G7:H7"/>
@@ -1546,7 +1597,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1562,24 +1613,24 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1587,24 +1638,24 @@
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1612,24 +1663,24 @@
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1637,24 +1688,24 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1662,24 +1713,24 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1687,126 +1738,126 @@
         <v>6</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="B14" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="B14" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="B15" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="B15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>96</v>
+      <c r="B18" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="G22" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="12"/>
+      <c r="B22" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="G22" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="G23" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H23" s="14"/>
+      <c r="B23" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="G23" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="15"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="11" t="s">
+      <c r="B25" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="13" customHeight="1">
+      <c r="B26" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="13" customHeight="1">
+      <c r="B27" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="13" customHeight="1">
+      <c r="B28" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="13" customHeight="1">
-      <c r="B26" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" s="11" t="s">
+      <c r="C28" s="12" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" ht="13" customHeight="1">
-      <c r="B27" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="13" customHeight="1">
-      <c r="B28" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>135</v>
+      <c r="G28" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="13" customHeight="1"/>

</xml_diff>